<commit_message>
add copo_name for study.title
</commit_message>
<xml_diff>
--- a/single_cell/singlecell_schema_main_v0.2.xlsx
+++ b/single_cell/singlecell_schema_main_v0.2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/providen/Documents/EI/Projects/SingleCellSchemas/schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zef22hak/development/COPO-schemas/single_cell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6ED588-95AE-F443-B514-5D87EBEA0B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C6587F-F8DD-9C4F-B491-43CB08E2EC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" xr2:uid="{7BD8D0E6-E1F4-E04F-9790-31602B31B6DB}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4074" uniqueCount="1789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4077" uniqueCount="1789">
   <si>
     <t>component_name</t>
   </si>
@@ -7096,10 +7096,10 @@
   </sheetPr>
   <dimension ref="A1:X196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="U1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A23" sqref="A23"/>
-      <selection pane="topRight" activeCell="V30" sqref="V30"/>
+      <selection pane="topRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7283,6 +7283,9 @@
       <c r="D3" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
       </c>
@@ -7340,6 +7343,9 @@
       </c>
       <c r="D4" s="3" t="s">
         <v>45</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
@@ -9003,7 +9009,7 @@
       <c r="S31" s="61"/>
       <c r="T31" s="90"/>
       <c r="U31" s="91" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="V31" s="92"/>
       <c r="W31" s="93"/>
@@ -9625,13 +9631,11 @@
       <c r="R43" s="10"/>
       <c r="S43" s="15"/>
       <c r="T43" s="11"/>
-      <c r="U43" s="12" t="s">
-        <v>35</v>
-      </c>
+      <c r="U43" s="12"/>
       <c r="V43" s="13"/>
       <c r="W43" s="14"/>
       <c r="X43" s="68" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -38061,10 +38065,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38201,6 +38205,14 @@
         <v>1787</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>